<commit_message>
Added course data. Added resources. Updated Friday's meetup time.
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbryer/Dropbox (SPS)/Teaching/DATA606 2022 Spring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4573A43-78A7-E641-8207-720C79D88C2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45637A31-7752-464F-80C3-57BFDE3C783A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20560" yWindow="8080" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
   </bookViews>
   <sheets>
     <sheet name="Meetups" sheetId="1" r:id="rId1"/>
@@ -197,12 +197,6 @@
     <t>Spring Break</t>
   </si>
   <si>
-    <t>1pm</t>
-  </si>
-  <si>
-    <t>2pm</t>
-  </si>
-  <si>
     <t>Chapter 1 - Intro to Data, R, and RStudio</t>
   </si>
   <si>
@@ -210,6 +204,12 @@
   </si>
   <si>
     <t>/assesssments/midterm/</t>
+  </si>
+  <si>
+    <t>2:30 pm</t>
+  </si>
+  <si>
+    <t>3:30 pm</t>
   </si>
 </sst>
 </file>
@@ -591,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA12B6D5-EAC3-1C40-AC8A-3C6A227098E4}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -629,10 +629,10 @@
         <v>44589</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D2" t="s">
         <v>46</v>
@@ -908,8 +908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD67FB80-52EB-7F41-88A6-58F30ED23B0C}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -941,7 +941,7 @@
         <v>44598</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
@@ -1011,10 +1011,10 @@
         <v>44635</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added intro to course slides.
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbryer/Dropbox (SPS)/Teaching/DATA606 2022 Spring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45637A31-7752-464F-80C3-57BFDE3C783A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E2DDA3-1CDA-6448-98F7-50B47BBD5F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
+    <workbookView xWindow="19300" yWindow="9160" windowWidth="28800" windowHeight="17500" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
   </bookViews>
   <sheets>
     <sheet name="Meetups" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="61">
   <si>
     <t>Date</t>
   </si>
@@ -210,6 +210,15 @@
   </si>
   <si>
     <t>3:30 pm</t>
+  </si>
+  <si>
+    <t>Youtube</t>
+  </si>
+  <si>
+    <t>Slides</t>
+  </si>
+  <si>
+    <t>00-Intro_to_Course</t>
   </si>
 </sst>
 </file>
@@ -589,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA12B6D5-EAC3-1C40-AC8A-3C6A227098E4}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -601,10 +610,11 @@
     <col min="2" max="3" width="18.5" style="3" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="33.5" customWidth="1"/>
+    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -621,10 +631,16 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>44589</v>
       </c>
@@ -640,8 +656,11 @@
       <c r="E2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>44594</v>
       </c>
@@ -658,7 +677,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>44601</v>
       </c>
@@ -675,7 +694,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>44608</v>
       </c>
@@ -692,7 +711,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>44615</v>
       </c>
@@ -708,9 +727,9 @@
       <c r="E6" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="6"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>44622</v>
       </c>
@@ -726,9 +745,9 @@
       <c r="E7" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>44629</v>
       </c>
@@ -744,9 +763,9 @@
       <c r="E8" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="6"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>44636</v>
       </c>
@@ -762,9 +781,9 @@
       <c r="E9" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>44643</v>
       </c>
@@ -780,9 +799,9 @@
       <c r="E10" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="6"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>44650</v>
       </c>
@@ -798,9 +817,9 @@
       <c r="E11" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="6"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>44657</v>
       </c>
@@ -816,9 +835,9 @@
       <c r="E12" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>44664</v>
       </c>
@@ -834,18 +853,18 @@
       <c r="E13" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="6"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>44671</v>
       </c>
       <c r="D14" t="s">
         <v>51</v>
       </c>
-      <c r="F14" s="6"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H14" s="6"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>44678</v>
       </c>
@@ -861,9 +880,9 @@
       <c r="E15" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="6"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>44685</v>
       </c>
@@ -879,7 +898,7 @@
       <c r="E16" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="6"/>
+      <c r="H16" s="6"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1">

</xml_diff>

<commit_message>
Added intro to course video.
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbryer/Dropbox (SPS)/Teaching/DATA606 2022 Spring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E2DDA3-1CDA-6448-98F7-50B47BBD5F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F0FD18-702D-074F-B8E3-A3CAC66CB55C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19300" yWindow="9160" windowWidth="28800" windowHeight="17500" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="62">
   <si>
     <t>Date</t>
   </si>
@@ -219,6 +219,9 @@
   </si>
   <si>
     <t>00-Intro_to_Course</t>
+  </si>
+  <si>
+    <t>CWydtLn7n6o</t>
   </si>
 </sst>
 </file>
@@ -601,7 +604,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -610,6 +613,7 @@
     <col min="2" max="3" width="18.5" style="3" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.1640625" customWidth="1"/>
   </cols>
@@ -655,6 +659,9 @@
       </c>
       <c r="E2" t="s">
         <v>29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>61</v>
       </c>
       <c r="G2" t="s">
         <v>60</v>

</xml_diff>

<commit_message>
Added R Package development talk materials.
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbryer/Dropbox (SPS)/Teaching/DATA606 2022 Spring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D722CFE-D429-2648-8C93-80B99BBCD6C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A5FDFC-9954-B342-9547-6F14E4873B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16820" yWindow="9460" windowWidth="28800" windowHeight="17500" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="78">
   <si>
     <t>Date</t>
   </si>
@@ -255,6 +255,22 @@
   </si>
   <si>
     <t>04-Distributions</t>
+  </si>
+  <si>
+    <t>7:00 pm</t>
+  </si>
+  <si>
+    <t>R Package Development</t>
+  </si>
+  <si>
+    <t>vlyVKGSVCsk</t>
+  </si>
+  <si>
+    <t>2022-03-01-R_Package_Development</t>
+  </si>
+  <si>
+    <t>R script located here: https://github.com/jbryer/DATA606Spring2022/blob/main/Slides/2022-03-01-R_Package_Development/Build_R_Package.R
+You can download the supporting materials here: https://github.com/jbryer/DATA606Spring2022/blob/main/Slides/2022-03-01-R_Package_Development/</t>
   </si>
 </sst>
 </file>
@@ -302,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -320,6 +336,9 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -634,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA12B6D5-EAC3-1C40-AC8A-3C6A227098E4}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -647,7 +666,7 @@
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" customWidth="1"/>
-    <col min="7" max="7" width="19.83203125" customWidth="1"/>
+    <col min="7" max="7" width="33.6640625" customWidth="1"/>
     <col min="8" max="8" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -796,36 +815,41 @@
       </c>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>44622</v>
+        <v>44621</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" s="6"/>
+        <v>74</v>
+      </c>
+      <c r="F7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G7" t="s">
+        <v>76</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>44629</v>
+        <v>44622</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E8" t="s">
         <v>29</v>
@@ -834,7 +858,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>44636</v>
+        <v>44629</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>11</v>
@@ -843,7 +867,7 @@
         <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="E9" t="s">
         <v>29</v>
@@ -852,7 +876,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>44643</v>
+        <v>44636</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>11</v>
@@ -861,7 +885,7 @@
         <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E10" t="s">
         <v>29</v>
@@ -870,7 +894,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>44650</v>
+        <v>44643</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>11</v>
@@ -879,7 +903,7 @@
         <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
         <v>29</v>
@@ -888,7 +912,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>44657</v>
+        <v>44650</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>11</v>
@@ -897,7 +921,7 @@
         <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E12" t="s">
         <v>29</v>
@@ -906,7 +930,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>44664</v>
+        <v>44657</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>11</v>
@@ -915,7 +939,7 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E13" t="s">
         <v>29</v>
@@ -924,34 +948,34 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>44671</v>
+        <v>44664</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
+        <v>42</v>
+      </c>
+      <c r="E14" t="s">
+        <v>29</v>
       </c>
       <c r="H14" s="6"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>44678</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>12</v>
+        <v>44671</v>
       </c>
       <c r="D15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="H15" s="6"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>44685</v>
+        <v>44678</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>11</v>
@@ -960,16 +984,16 @@
         <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E16" t="s">
         <v>29</v>
       </c>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>44692</v>
+        <v>44685</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>11</v>
@@ -978,9 +1002,27 @@
         <v>12</v>
       </c>
       <c r="D17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>44692</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" t="s">
         <v>45</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E18" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>